<commit_message>
all factures in one xml file
</commit_message>
<xml_diff>
--- a/FACTURES/doklady-CZ-06_2021-DPH.xlsx
+++ b/FACTURES/doklady-CZ-06_2021-DPH.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PYTHON\PROJECTS\XML_app\XML_app\FACTURES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tkminek_local\PYTHON\XML_FILE\XML_app\FACTURES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3208680-58F9-4A00-994A-6B88310029DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6444" yWindow="1860" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6450" yWindow="1860" windowWidth="17280" windowHeight="8970" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="EK 15%" sheetId="12" r:id="rId1"/>
@@ -33,12 +32,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'VK 21%'!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'VK RCH'!$A$1:$U$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="153">
   <si>
     <t>CZK</t>
   </si>
@@ -502,7 +501,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
@@ -1082,8 +1081,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Čárka" xfId="1" builtinId="3"/>
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1121,7 +1120,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1196,23 +1195,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1248,23 +1230,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1440,35 +1405,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="74" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.88671875" style="74" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="74" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="74" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5" style="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.6640625" style="7"/>
+    <col min="17" max="16384" width="10.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
         <v>19</v>
       </c>
@@ -1510,7 +1475,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="102"/>
       <c r="B2" s="101"/>
       <c r="C2" s="101"/>
@@ -1528,7 +1493,7 @@
       <c r="O2" s="101"/>
       <c r="P2" s="101"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="102"/>
       <c r="B3" s="101"/>
       <c r="C3" s="101"/>
@@ -1546,7 +1511,7 @@
       <c r="O3" s="101"/>
       <c r="P3" s="101"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M4" s="92" t="s">
         <v>18</v>
       </c>
@@ -1558,7 +1523,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1569,32 +1534,32 @@
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.44140625" style="64" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" style="64" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="51" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="63" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.6640625" style="63" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" style="64" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" style="99" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.44140625" style="64" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" style="99" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.44140625" style="64" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.109375" style="65" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" style="63" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="64" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="99" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" style="64" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="99" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" style="64" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" style="65" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2" style="65" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" style="65" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.44140625" style="64" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="65" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" style="64" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" style="36" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5" style="36" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8" style="36" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="10.33203125" style="36"/>
-    <col min="20" max="20" width="14.33203125" style="36" customWidth="1"/>
-    <col min="21" max="21" width="14.109375" style="36" customWidth="1"/>
-    <col min="22" max="16384" width="10.33203125" style="36"/>
+    <col min="18" max="19" width="10.28515625" style="36"/>
+    <col min="20" max="20" width="14.28515625" style="36" customWidth="1"/>
+    <col min="21" max="21" width="14.140625" style="36" customWidth="1"/>
+    <col min="22" max="16384" width="10.28515625" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="113" t="s">
         <v>19</v>
       </c>
@@ -1655,7 +1620,7 @@
       </c>
       <c r="W1" s="124"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="114" t="s">
         <v>58</v>
       </c>
@@ -1722,7 +1687,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="114" t="s">
         <v>79</v>
       </c>
@@ -1789,7 +1754,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>55</v>
       </c>
@@ -1857,7 +1822,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="114" t="s">
         <v>71</v>
       </c>
@@ -1924,7 +1889,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="114" t="s">
         <v>84</v>
       </c>
@@ -1991,7 +1956,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="114" t="s">
         <v>89</v>
       </c>
@@ -2058,7 +2023,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="114" t="s">
         <v>89</v>
       </c>
@@ -2125,7 +2090,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="114" t="s">
         <v>89</v>
       </c>
@@ -2192,7 +2157,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="114" t="s">
         <v>89</v>
       </c>
@@ -2259,7 +2224,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I11" s="99">
         <f>SUM(I2:I10)</f>
         <v>-1011597.14</v>
@@ -2269,7 +2234,7 @@
         <v>-25642292.967700001</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="128" t="s">
         <v>147</v>
       </c>
@@ -2278,7 +2243,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V10">
+  <sortState ref="A2:V10">
     <sortCondition ref="S2:S10"/>
   </sortState>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2287,7 +2252,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
@@ -2298,20 +2263,20 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.6640625" style="15"/>
+    <col min="1" max="1" width="10.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.7109375" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>6</v>
       </c>
@@ -2352,7 +2317,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="61" t="s">
         <v>131</v>
       </c>
@@ -2394,7 +2359,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>46</v>
       </c>
@@ -2421,7 +2386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -2434,7 +2399,7 @@
       </c>
       <c r="H4" s="22"/>
     </row>
-    <row r="5" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -2444,7 +2409,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="22"/>
     </row>
-    <row r="6" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -2454,7 +2419,7 @@
       <c r="G6" s="6"/>
       <c r="H6" s="22"/>
     </row>
-    <row r="7" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -2464,7 +2429,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="22"/>
     </row>
-    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="76" t="s">
         <v>48</v>
       </c>
@@ -2491,7 +2456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="61" t="s">
         <v>44</v>
       </c>
@@ -2518,7 +2483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="61" t="s">
         <v>39</v>
       </c>
@@ -2545,7 +2510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G11" s="92">
         <f>SUM(G8:G10)</f>
         <v>0</v>
@@ -2558,7 +2523,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2568,23 +2533,23 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="59" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="60" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.5546875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="60" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.5703125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" style="7" customWidth="1"/>
     <col min="11" max="11" width="12" style="7" customWidth="1"/>
-    <col min="12" max="16384" width="15.109375" style="7"/>
+    <col min="12" max="16384" width="15.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
         <v>16</v>
       </c>
@@ -2601,7 +2566,7 @@
       <c r="J1" s="30"/>
       <c r="K1" s="32"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="33">
         <v>44348</v>
       </c>
@@ -2618,7 +2583,7 @@
       <c r="J2" s="36"/>
       <c r="K2" s="39"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>11</v>
       </c>
@@ -2635,7 +2600,7 @@
       <c r="J3" s="36"/>
       <c r="K3" s="39"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="40"/>
       <c r="B4" s="34"/>
       <c r="C4" s="35"/>
@@ -2648,7 +2613,7 @@
       <c r="J4" s="36"/>
       <c r="K4" s="39"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="42" t="s">
         <v>3</v>
       </c>
@@ -2669,7 +2634,7 @@
       </c>
       <c r="K5" s="26"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="44">
         <v>0</v>
       </c>
@@ -2698,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="44">
         <v>0.15</v>
       </c>
@@ -2727,7 +2692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="44">
         <v>0.21</v>
       </c>
@@ -2756,7 +2721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="40"/>
       <c r="B9" s="47">
         <f>SUM(B7:B8)</f>
@@ -2781,7 +2746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="40"/>
       <c r="B10" s="34"/>
       <c r="C10" s="35"/>
@@ -2794,7 +2759,7 @@
       <c r="J10" s="36"/>
       <c r="K10" s="39"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="40"/>
       <c r="B11" s="34"/>
       <c r="C11" s="35"/>
@@ -2807,7 +2772,7 @@
       <c r="J11" s="36"/>
       <c r="K11" s="39"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="40"/>
       <c r="B12" s="34"/>
       <c r="C12" s="50">
@@ -2830,7 +2795,7 @@
       </c>
       <c r="K12" s="39"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
       <c r="B13" s="34"/>
       <c r="C13" s="35"/>
@@ -2843,7 +2808,7 @@
       <c r="J13" s="36"/>
       <c r="K13" s="39"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="40"/>
       <c r="B14" s="34"/>
       <c r="C14" s="35"/>
@@ -2856,7 +2821,7 @@
       <c r="J14" s="36"/>
       <c r="K14" s="39"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
         <v>2</v>
       </c>
@@ -2885,7 +2850,7 @@
         <v>1011597.14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="42" t="s">
         <v>15</v>
       </c>
@@ -2914,7 +2879,7 @@
         <v>3259367.39</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="42" t="s">
         <v>42</v>
       </c>
@@ -2943,7 +2908,7 @@
         <v>260371.04</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="42" t="s">
         <v>5</v>
       </c>
@@ -2972,7 +2937,7 @@
         <v>11285.31</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="52"/>
       <c r="B19" s="53">
         <f>SUM(B15:B18)</f>
@@ -2997,7 +2962,7 @@
         <v>4542620.88</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="74"/>
     </row>
   </sheetData>
@@ -3007,35 +2972,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3" style="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5" style="11" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.5546875" style="11"/>
+    <col min="17" max="16384" width="11.5703125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="82" t="s">
         <v>19</v>
       </c>
@@ -3077,7 +3042,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="83"/>
       <c r="B2" s="82"/>
       <c r="C2" s="82"/>
@@ -3095,7 +3060,7 @@
       <c r="O2" s="82"/>
       <c r="P2" s="82"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="C3" s="11"/>
       <c r="E3" s="11"/>
@@ -3103,7 +3068,7 @@
       <c r="K3" s="1"/>
       <c r="M3" s="12"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="C4" s="11"/>
       <c r="E4" s="11"/>
@@ -3111,7 +3076,7 @@
       <c r="K4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="C5" s="11"/>
       <c r="E5" s="11"/>
@@ -3122,7 +3087,7 @@
       <c r="K5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="C6" s="11"/>
       <c r="E6" s="11"/>
@@ -3130,7 +3095,7 @@
       <c r="K6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="C7" s="11"/>
       <c r="E7" s="11"/>
@@ -3138,7 +3103,7 @@
       <c r="K7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="C8" s="11"/>
       <c r="E8" s="11"/>
@@ -3146,7 +3111,7 @@
       <c r="K8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="C9" s="11"/>
       <c r="E9" s="11"/>
@@ -3154,7 +3119,7 @@
       <c r="K9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="C10" s="11"/>
       <c r="E10" s="11"/>
@@ -3162,7 +3127,7 @@
       <c r="K10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="C11" s="11"/>
       <c r="E11" s="11"/>
@@ -3170,7 +3135,7 @@
       <c r="K11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="C12" s="11"/>
       <c r="E12" s="11"/>
@@ -3178,7 +3143,7 @@
       <c r="K12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="C13" s="11"/>
       <c r="E13" s="11"/>
@@ -3186,7 +3151,7 @@
       <c r="K13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="C14" s="11"/>
       <c r="E14" s="11"/>
@@ -3194,7 +3159,7 @@
       <c r="K14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="C15" s="11"/>
       <c r="E15" s="11"/>
@@ -3202,7 +3167,7 @@
       <c r="K15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="C16" s="11"/>
       <c r="E16" s="11"/>
@@ -3210,7 +3175,7 @@
       <c r="K16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="C17" s="11"/>
       <c r="E17" s="11"/>
@@ -3218,7 +3183,7 @@
       <c r="K17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="C18" s="11"/>
       <c r="E18" s="11"/>
@@ -3226,7 +3191,7 @@
       <c r="K18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="C19" s="11"/>
       <c r="E19" s="11"/>
@@ -3234,7 +3199,7 @@
       <c r="K19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="C20" s="11"/>
       <c r="E20" s="11"/>
@@ -3242,7 +3207,7 @@
       <c r="K20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="C21" s="11"/>
       <c r="E21" s="11"/>
@@ -3250,7 +3215,7 @@
       <c r="K21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="C22" s="11"/>
       <c r="E22" s="11"/>
@@ -3258,7 +3223,7 @@
       <c r="K22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="C23" s="11"/>
       <c r="E23" s="11"/>
@@ -3266,7 +3231,7 @@
       <c r="K23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="C24" s="11"/>
       <c r="E24" s="11"/>
@@ -3274,7 +3239,7 @@
       <c r="K24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="C25" s="11"/>
       <c r="E25" s="11"/>
@@ -3282,7 +3247,7 @@
       <c r="K25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="C26" s="11"/>
       <c r="E26" s="11"/>
@@ -3290,7 +3255,7 @@
       <c r="K26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="C27" s="11"/>
       <c r="E27" s="11"/>
@@ -3298,7 +3263,7 @@
       <c r="K27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="C28" s="11"/>
       <c r="E28" s="11"/>
@@ -3306,7 +3271,7 @@
       <c r="K28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="C29" s="11"/>
       <c r="E29" s="11"/>
@@ -3314,7 +3279,7 @@
       <c r="K29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="C30" s="11"/>
       <c r="E30" s="11"/>
@@ -3322,7 +3287,7 @@
       <c r="K30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="C31" s="11"/>
       <c r="E31" s="11"/>
@@ -3330,7 +3295,7 @@
       <c r="K31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="C32" s="11"/>
       <c r="E32" s="11"/>
@@ -3338,7 +3303,7 @@
       <c r="K32" s="1"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="C33" s="11"/>
       <c r="E33" s="11"/>
@@ -3346,7 +3311,7 @@
       <c r="K33" s="1"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="C34" s="11"/>
       <c r="E34" s="11"/>
@@ -3354,7 +3319,7 @@
       <c r="K34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="C35" s="11"/>
       <c r="E35" s="11"/>
@@ -3362,7 +3327,7 @@
       <c r="K35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="C36" s="11"/>
       <c r="E36" s="11"/>
@@ -3370,7 +3335,7 @@
       <c r="K36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="C37" s="11"/>
       <c r="E37" s="11"/>
@@ -3378,7 +3343,7 @@
       <c r="K37" s="1"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="C38" s="11"/>
       <c r="E38" s="11"/>
@@ -3386,7 +3351,7 @@
       <c r="K38" s="1"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="C39" s="11"/>
       <c r="E39" s="11"/>
@@ -3394,7 +3359,7 @@
       <c r="K39" s="1"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="C40" s="11"/>
       <c r="E40" s="11"/>
@@ -3402,7 +3367,7 @@
       <c r="K40" s="1"/>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="C41" s="11"/>
       <c r="E41" s="11"/>
@@ -3410,7 +3375,7 @@
       <c r="K41" s="1"/>
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="C42" s="11"/>
       <c r="E42" s="11"/>
@@ -3418,7 +3383,7 @@
       <c r="K42" s="1"/>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="C43" s="11"/>
       <c r="E43" s="11"/>
@@ -3426,7 +3391,7 @@
       <c r="K43" s="1"/>
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="C44" s="11"/>
       <c r="E44" s="11"/>
@@ -3434,7 +3399,7 @@
       <c r="K44" s="1"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="C45" s="11"/>
       <c r="E45" s="11"/>
@@ -3442,7 +3407,7 @@
       <c r="K45" s="1"/>
       <c r="M45" s="1"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="C46" s="11"/>
       <c r="E46" s="11"/>
@@ -3450,7 +3415,7 @@
       <c r="K46" s="1"/>
       <c r="M46" s="1"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="C47" s="11"/>
       <c r="E47" s="11"/>
@@ -3458,7 +3423,7 @@
       <c r="K47" s="1"/>
       <c r="M47" s="1"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="C48" s="11"/>
       <c r="E48" s="11"/>
@@ -3466,7 +3431,7 @@
       <c r="K48" s="1"/>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="C49" s="11"/>
       <c r="E49" s="11"/>
@@ -3474,7 +3439,7 @@
       <c r="K49" s="1"/>
       <c r="M49" s="1"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="C50" s="11"/>
       <c r="E50" s="11"/>
@@ -3482,7 +3447,7 @@
       <c r="K50" s="1"/>
       <c r="M50" s="1"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="C51" s="11"/>
       <c r="E51" s="11"/>
@@ -3490,7 +3455,7 @@
       <c r="K51" s="1"/>
       <c r="M51" s="1"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="C52" s="11"/>
       <c r="E52" s="11"/>
@@ -3498,7 +3463,7 @@
       <c r="K52" s="1"/>
       <c r="M52" s="1"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="C53" s="11"/>
       <c r="E53" s="11"/>
@@ -3506,7 +3471,7 @@
       <c r="K53" s="1"/>
       <c r="M53" s="1"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="C54" s="11"/>
       <c r="E54" s="11"/>
@@ -3514,7 +3479,7 @@
       <c r="K54" s="1"/>
       <c r="M54" s="1"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="C55" s="11"/>
       <c r="E55" s="11"/>
@@ -3522,7 +3487,7 @@
       <c r="K55" s="1"/>
       <c r="M55" s="1"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="C56" s="11"/>
       <c r="E56" s="11"/>
@@ -3530,7 +3495,7 @@
       <c r="K56" s="1"/>
       <c r="M56" s="1"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="C57" s="11"/>
       <c r="E57" s="11"/>
@@ -3538,7 +3503,7 @@
       <c r="K57" s="1"/>
       <c r="M57" s="1"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="C58" s="11"/>
       <c r="E58" s="11"/>
@@ -3546,7 +3511,7 @@
       <c r="K58" s="1"/>
       <c r="M58" s="1"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="C59" s="11"/>
       <c r="E59" s="11"/>
@@ -3554,7 +3519,7 @@
       <c r="K59" s="1"/>
       <c r="M59" s="1"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="C60" s="11"/>
       <c r="E60" s="11"/>
@@ -3562,7 +3527,7 @@
       <c r="K60" s="1"/>
       <c r="M60" s="1"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="C61" s="11"/>
       <c r="E61" s="11"/>
@@ -3570,7 +3535,7 @@
       <c r="K61" s="1"/>
       <c r="M61" s="1"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="C62" s="11"/>
       <c r="E62" s="11"/>
@@ -3578,7 +3543,7 @@
       <c r="K62" s="1"/>
       <c r="M62" s="1"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="C63" s="11"/>
       <c r="E63" s="11"/>
@@ -3586,7 +3551,7 @@
       <c r="K63" s="1"/>
       <c r="M63" s="1"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="C64" s="11"/>
       <c r="E64" s="11"/>
@@ -3594,7 +3559,7 @@
       <c r="K64" s="1"/>
       <c r="M64" s="1"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="C65" s="11"/>
       <c r="E65" s="11"/>
@@ -3602,7 +3567,7 @@
       <c r="K65" s="1"/>
       <c r="M65" s="1"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="C66" s="11"/>
       <c r="E66" s="11"/>
@@ -3610,7 +3575,7 @@
       <c r="K66" s="1"/>
       <c r="M66" s="1"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="C67" s="11"/>
       <c r="E67" s="11"/>
@@ -3618,7 +3583,7 @@
       <c r="K67" s="1"/>
       <c r="M67" s="1"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="C68" s="11"/>
       <c r="E68" s="11"/>
@@ -3626,7 +3591,7 @@
       <c r="K68" s="1"/>
       <c r="M68" s="1"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="C69" s="11"/>
       <c r="E69" s="11"/>
@@ -3634,7 +3599,7 @@
       <c r="K69" s="1"/>
       <c r="M69" s="1"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="C70" s="11"/>
       <c r="E70" s="11"/>
@@ -3642,7 +3607,7 @@
       <c r="K70" s="1"/>
       <c r="M70" s="1"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="C71" s="11"/>
       <c r="E71" s="11"/>
@@ -3650,7 +3615,7 @@
       <c r="K71" s="1"/>
       <c r="M71" s="1"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="C72" s="11"/>
       <c r="E72" s="11"/>
@@ -3658,7 +3623,7 @@
       <c r="K72" s="1"/>
       <c r="M72" s="1"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="C73" s="11"/>
       <c r="E73" s="11"/>
@@ -3666,7 +3631,7 @@
       <c r="K73" s="1"/>
       <c r="M73" s="1"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="C74" s="11"/>
       <c r="E74" s="11"/>
@@ -3674,7 +3639,7 @@
       <c r="K74" s="1"/>
       <c r="M74" s="1"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="C75" s="11"/>
       <c r="E75" s="11"/>
@@ -3682,7 +3647,7 @@
       <c r="K75" s="1"/>
       <c r="M75" s="1"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="C76" s="11"/>
       <c r="E76" s="11"/>
@@ -3690,7 +3655,7 @@
       <c r="K76" s="1"/>
       <c r="M76" s="1"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="C77" s="11"/>
       <c r="E77" s="11"/>
@@ -3698,7 +3663,7 @@
       <c r="K77" s="1"/>
       <c r="M77" s="1"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="C78" s="11"/>
       <c r="E78" s="11"/>
@@ -3706,7 +3671,7 @@
       <c r="K78" s="1"/>
       <c r="M78" s="1"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="C79" s="11"/>
       <c r="E79" s="11"/>
@@ -3714,7 +3679,7 @@
       <c r="K79" s="1"/>
       <c r="M79" s="1"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="C80" s="11"/>
       <c r="E80" s="11"/>
@@ -3722,7 +3687,7 @@
       <c r="K80" s="1"/>
       <c r="M80" s="1"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="C81" s="11"/>
       <c r="E81" s="11"/>
@@ -3730,7 +3695,7 @@
       <c r="K81" s="1"/>
       <c r="M81" s="1"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="C82" s="11"/>
       <c r="E82" s="11"/>
@@ -3738,7 +3703,7 @@
       <c r="K82" s="1"/>
       <c r="M82" s="1"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="C83" s="11"/>
       <c r="E83" s="11"/>
@@ -3753,35 +3718,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1">
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="T53" sqref="T53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="90" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="51" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" style="63" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="79" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.44140625" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="79" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.44140625" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="90" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" style="63" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="79" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="79" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" style="35" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3" style="35" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="11.5546875" style="35"/>
+    <col min="13" max="16384" width="11.5703125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="105" t="s">
         <v>19</v>
       </c>
@@ -3823,7 +3788,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="129" t="s">
         <v>55</v>
       </c>
@@ -3870,7 +3835,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="129" t="s">
         <v>58</v>
       </c>
@@ -3917,7 +3882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="129" t="s">
         <v>55</v>
       </c>
@@ -3964,7 +3929,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="129" t="s">
         <v>55</v>
       </c>
@@ -4011,7 +3976,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="129" t="s">
         <v>55</v>
       </c>
@@ -4058,7 +4023,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="129" t="s">
         <v>55</v>
       </c>
@@ -4105,7 +4070,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="129" t="s">
         <v>55</v>
       </c>
@@ -4152,7 +4117,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="129" t="s">
         <v>57</v>
       </c>
@@ -4199,7 +4164,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="129" t="s">
         <v>58</v>
       </c>
@@ -4246,7 +4211,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="129" t="s">
         <v>61</v>
       </c>
@@ -4293,7 +4258,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="129" t="s">
         <v>67</v>
       </c>
@@ -4340,7 +4305,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="129" t="s">
         <v>69</v>
       </c>
@@ -4387,7 +4352,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="129" t="s">
         <v>69</v>
       </c>
@@ -4434,9 +4399,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="133">
-        <v>44351</v>
+    <row r="15" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="133" t="s">
+        <v>57</v>
       </c>
       <c r="B15" s="134" t="s">
         <v>30</v>
@@ -4480,8 +4445,11 @@
       <c r="O15" s="134">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P15" s="132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="133" t="s">
         <v>57</v>
       </c>
@@ -4528,10 +4496,10 @@
         <v>12</v>
       </c>
       <c r="P16" s="132">
-        <v>123456789</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" s="132" customFormat="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="133" t="s">
         <v>58</v>
       </c>
@@ -4577,8 +4545,11 @@
       <c r="O17" s="134">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" s="132" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P17" s="132">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="133" t="s">
         <v>58</v>
       </c>
@@ -4624,8 +4595,11 @@
       <c r="O18" s="134">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" s="132" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P18" s="132">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="133" t="s">
         <v>61</v>
       </c>
@@ -4671,8 +4645,11 @@
       <c r="O19" s="134">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" s="132" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P19" s="132">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="133" t="s">
         <v>61</v>
       </c>
@@ -4718,8 +4695,11 @@
       <c r="O20" s="134">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" s="132" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P20" s="132">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="133" t="s">
         <v>63</v>
       </c>
@@ -4765,8 +4745,11 @@
       <c r="O21" s="134">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" s="132" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P21" s="132">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="133" t="s">
         <v>63</v>
       </c>
@@ -4812,8 +4795,11 @@
       <c r="O22" s="134">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" s="132" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P22" s="132">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="133" t="s">
         <v>66</v>
       </c>
@@ -4859,8 +4845,11 @@
       <c r="O23" s="134">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" s="132" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P23" s="132">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="133" t="s">
         <v>67</v>
       </c>
@@ -4906,8 +4895,11 @@
       <c r="O24" s="134">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" s="132" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P24" s="132">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="133" t="s">
         <v>67</v>
       </c>
@@ -4953,8 +4945,11 @@
       <c r="O25" s="134">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" s="132" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P25" s="132">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="133" t="s">
         <v>67</v>
       </c>
@@ -5000,8 +4995,11 @@
       <c r="O26" s="134">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" s="132" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P26" s="132">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="133" t="s">
         <v>69</v>
       </c>
@@ -5047,8 +5045,11 @@
       <c r="O27" s="134">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" s="132" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P27" s="132">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="133" t="s">
         <v>69</v>
       </c>
@@ -5094,8 +5095,11 @@
       <c r="O28" s="134">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" s="132" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P28" s="132">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="133" t="s">
         <v>71</v>
       </c>
@@ -5141,8 +5145,11 @@
       <c r="O29" s="134">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" s="132" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P29" s="132">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="133" t="s">
         <v>71</v>
       </c>
@@ -5188,8 +5195,11 @@
       <c r="O30" s="134">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P30" s="132">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="106" t="s">
         <v>72</v>
       </c>
@@ -5235,8 +5245,11 @@
       <c r="O31" s="105">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P31" s="132">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="106" t="s">
         <v>72</v>
       </c>
@@ -5282,8 +5295,11 @@
       <c r="O32" s="105">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P32" s="132">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="106" t="s">
         <v>72</v>
       </c>
@@ -5329,8 +5345,11 @@
       <c r="O33" s="105">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P33" s="132">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="106" t="s">
         <v>72</v>
       </c>
@@ -5376,8 +5395,11 @@
       <c r="O34" s="105">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P34" s="132">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="106" t="s">
         <v>75</v>
       </c>
@@ -5423,8 +5445,11 @@
       <c r="O35" s="105">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P35" s="132">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="106" t="s">
         <v>75</v>
       </c>
@@ -5470,8 +5495,11 @@
       <c r="O36" s="105">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P36" s="132">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="106" t="s">
         <v>75</v>
       </c>
@@ -5517,8 +5545,11 @@
       <c r="O37" s="105">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P37" s="132">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="106" t="s">
         <v>75</v>
       </c>
@@ -5564,8 +5595,11 @@
       <c r="O38" s="105">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P38" s="132">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="106" t="s">
         <v>75</v>
       </c>
@@ -5611,8 +5645,11 @@
       <c r="O39" s="105">
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P39" s="132">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="106" t="s">
         <v>77</v>
       </c>
@@ -5658,8 +5695,11 @@
       <c r="O40" s="105">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P40" s="132">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="114" t="s">
         <v>78</v>
       </c>
@@ -5705,8 +5745,11 @@
       <c r="O41" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P41" s="132">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="114" t="s">
         <v>79</v>
       </c>
@@ -5752,8 +5795,11 @@
       <c r="O42" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P42" s="132">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="114" t="s">
         <v>79</v>
       </c>
@@ -5799,8 +5845,11 @@
       <c r="O43" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P43" s="132">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="114" t="s">
         <v>79</v>
       </c>
@@ -5846,8 +5895,11 @@
       <c r="O44" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P44" s="132">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="114" t="s">
         <v>79</v>
       </c>
@@ -5893,8 +5945,11 @@
       <c r="O45" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P45" s="132">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="114" t="s">
         <v>80</v>
       </c>
@@ -5940,8 +5995,11 @@
       <c r="O46" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P46" s="132">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="114" t="s">
         <v>80</v>
       </c>
@@ -5987,8 +6045,11 @@
       <c r="O47" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P47" s="132">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="114" t="s">
         <v>81</v>
       </c>
@@ -6034,8 +6095,11 @@
       <c r="O48" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P48" s="132">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="114" t="s">
         <v>81</v>
       </c>
@@ -6081,8 +6145,11 @@
       <c r="O49" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P49" s="132">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="114" t="s">
         <v>83</v>
       </c>
@@ -6128,8 +6195,11 @@
       <c r="O50" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P50" s="132">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="114" t="s">
         <v>83</v>
       </c>
@@ -6175,8 +6245,11 @@
       <c r="O51" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P51" s="132">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="114" t="s">
         <v>84</v>
       </c>
@@ -6222,8 +6295,11 @@
       <c r="O52" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P52" s="132">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="114" t="s">
         <v>84</v>
       </c>
@@ -6269,8 +6345,11 @@
       <c r="O53" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P53" s="132">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="114" t="s">
         <v>84</v>
       </c>
@@ -6316,8 +6395,11 @@
       <c r="O54" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P54" s="132">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="114" t="s">
         <v>84</v>
       </c>
@@ -6363,8 +6445,11 @@
       <c r="O55" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P55" s="132">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="114" t="s">
         <v>84</v>
       </c>
@@ -6410,8 +6495,11 @@
       <c r="O56" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P56" s="132">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="114" t="s">
         <v>84</v>
       </c>
@@ -6457,8 +6545,11 @@
       <c r="O57" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P57" s="132">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="114" t="s">
         <v>87</v>
       </c>
@@ -6504,8 +6595,11 @@
       <c r="O58" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P58" s="132">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="114" t="s">
         <v>87</v>
       </c>
@@ -6551,8 +6645,11 @@
       <c r="O59" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P59" s="132">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="114" t="s">
         <v>87</v>
       </c>
@@ -6598,8 +6695,11 @@
       <c r="O60" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P60" s="132">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="114" t="s">
         <v>87</v>
       </c>
@@ -6645,8 +6745,11 @@
       <c r="O61" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P61" s="132">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="114" t="s">
         <v>89</v>
       </c>
@@ -6692,8 +6795,11 @@
       <c r="O62" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P62" s="132">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="114" t="s">
         <v>89</v>
       </c>
@@ -6739,8 +6845,11 @@
       <c r="O63" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P63" s="132">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="114" t="s">
         <v>89</v>
       </c>
@@ -6786,8 +6895,11 @@
       <c r="O64" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P64" s="132">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="114" t="s">
         <v>89</v>
       </c>
@@ -6833,8 +6945,11 @@
       <c r="O65" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P65" s="132">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="114" t="s">
         <v>89</v>
       </c>
@@ -6880,8 +6995,11 @@
       <c r="O66" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P66" s="132">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="114" t="s">
         <v>89</v>
       </c>
@@ -6927,8 +7045,11 @@
       <c r="O67" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P67" s="132">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="114" t="s">
         <v>89</v>
       </c>
@@ -6974,8 +7095,11 @@
       <c r="O68" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P68" s="132">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="114" t="s">
         <v>89</v>
       </c>
@@ -7021,20 +7145,23 @@
       <c r="O69" s="113">
         <v>12</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P69" s="132">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G70" s="115">
         <f>SUM(G15:G69)</f>
         <v>39745164.280000009</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:O70" xr:uid="{26B0F9C7-D48A-42D3-A373-5A4655A54844}">
+  <autoFilter ref="A2:O70">
     <filterColumn colId="14">
       <colorFilter dxfId="1" cellColor="0"/>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O69">
+  <sortState ref="A2:O69">
     <sortCondition sortBy="cellColor" ref="O69" dxfId="0"/>
   </sortState>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -7043,7 +7170,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
@@ -7054,29 +7181,29 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="89" customWidth="1"/>
-    <col min="2" max="2" width="3.109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="89" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="51" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="51" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" style="63" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" style="64" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" style="100" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.44140625" style="100" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="64" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.44140625" style="64" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.109375" style="64" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="64" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="100" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" style="100" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="64" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" style="64" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" style="64" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2" style="64" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" style="65" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" style="64" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="65" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" style="64" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" style="36" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5" style="36" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8" style="36" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="11.109375" style="36"/>
+    <col min="18" max="16384" width="11.140625" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="103" t="s">
         <v>19</v>
       </c>
@@ -7137,7 +7264,7 @@
       </c>
       <c r="W1" s="124"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="108" t="s">
         <v>58</v>
       </c>
@@ -7206,7 +7333,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="108" t="s">
         <v>75</v>
       </c>
@@ -7275,7 +7402,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="108" t="s">
         <v>75</v>
       </c>
@@ -7344,7 +7471,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="108" t="s">
         <v>78</v>
       </c>
@@ -7413,7 +7540,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="108" t="s">
         <v>78</v>
       </c>
@@ -7482,7 +7609,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="108" t="s">
         <v>78</v>
       </c>
@@ -7551,7 +7678,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="108" t="s">
         <v>78</v>
       </c>
@@ -7620,7 +7747,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="108" t="s">
         <v>78</v>
       </c>
@@ -7689,7 +7816,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="108" t="s">
         <v>97</v>
       </c>
@@ -7758,7 +7885,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="108" t="s">
         <v>97</v>
       </c>
@@ -7827,7 +7954,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I12" s="64">
         <f>SUM(I2:I11)</f>
         <v>1263840.33</v>
@@ -7844,7 +7971,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA203FA5-2D96-4BAA-9D92-3C9068204297}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -7854,16 +7981,16 @@
       <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="113" t="s">
         <v>19</v>
       </c>
@@ -7923,7 +8050,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="114" t="s">
         <v>58</v>
       </c>
@@ -7992,7 +8119,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="114" t="s">
         <v>78</v>
       </c>
@@ -8061,7 +8188,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="114" t="s">
         <v>97</v>
       </c>
@@ -8130,7 +8257,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="114"/>
       <c r="C5" s="91"/>
       <c r="D5" s="91"/>
@@ -8152,7 +8279,7 @@
       <c r="U5" s="36"/>
       <c r="V5" s="36"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="114" t="s">
         <v>75</v>
       </c>
@@ -8221,7 +8348,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="114" t="s">
         <v>75</v>
       </c>
@@ -8290,7 +8417,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="114" t="s">
         <v>78</v>
       </c>
@@ -8359,7 +8486,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="114" t="s">
         <v>78</v>
       </c>
@@ -8428,7 +8555,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="114" t="s">
         <v>78</v>
       </c>
@@ -8497,7 +8624,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="114" t="s">
         <v>78</v>
       </c>
@@ -8566,7 +8693,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="114" t="s">
         <v>97</v>
       </c>
@@ -8635,7 +8762,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="89"/>
       <c r="B13" s="36"/>
       <c r="C13" s="51"/>
@@ -8668,12 +8795,12 @@
       <c r="U13" s="36"/>
       <c r="V13" s="36"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="113" t="s">
         <v>19</v>
       </c>
@@ -8733,7 +8860,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="114" t="s">
         <v>58</v>
       </c>
@@ -8800,7 +8927,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="114" t="s">
         <v>79</v>
       </c>
@@ -8867,7 +8994,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="23" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="114"/>
       <c r="G23" s="114"/>
       <c r="I23" s="114"/>
@@ -8886,7 +9013,7 @@
       <c r="U23" s="36"/>
       <c r="V23" s="36"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>55</v>
       </c>
@@ -8954,7 +9081,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="126"/>
       <c r="C25" s="126"/>
@@ -8980,7 +9107,7 @@
       <c r="U25" s="36"/>
       <c r="V25" s="36"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="114" t="s">
         <v>71</v>
       </c>
@@ -9047,7 +9174,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="114" t="s">
         <v>84</v>
       </c>
@@ -9114,7 +9241,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="114" t="s">
         <v>89</v>
       </c>
@@ -9181,7 +9308,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="114"/>
       <c r="G29" s="114"/>
       <c r="I29" s="114"/>
@@ -9200,7 +9327,7 @@
       <c r="U29" s="36"/>
       <c r="V29" s="36"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="114" t="s">
         <v>89</v>
       </c>
@@ -9267,7 +9394,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="114"/>
       <c r="G31" s="114"/>
       <c r="I31" s="114"/>
@@ -9283,7 +9410,7 @@
       <c r="U31" s="36"/>
       <c r="V31" s="36"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="114" t="s">
         <v>89</v>
       </c>
@@ -9350,7 +9477,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="114" t="s">
         <v>89</v>
       </c>
@@ -9417,7 +9544,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="36"/>
       <c r="B34" s="64"/>
       <c r="C34" s="51"/>
@@ -9450,7 +9577,7 @@
       <c r="U34" s="36"/>
       <c r="V34" s="36"/>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="128" t="s">
         <v>147</v>
       </c>
@@ -9479,7 +9606,7 @@
       <c r="V35" s="36"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:V12">
+  <sortState ref="A3:V12">
     <sortCondition ref="S3:S12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -9488,7 +9615,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
@@ -9499,25 +9626,25 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" style="114" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" style="114" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="114" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="114" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" style="80" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2" style="80" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="109" t="s">
         <v>19</v>
       </c>
@@ -9556,7 +9683,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="110" t="s">
         <v>55</v>
       </c>
@@ -9608,35 +9735,35 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5" style="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.109375" style="7"/>
+    <col min="17" max="16384" width="11.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="97" t="s">
         <v>19</v>
       </c>
@@ -9678,7 +9805,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F5" s="92" t="s">
         <v>18</v>
       </c>
@@ -9690,31 +9817,31 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" style="86" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="86" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3" style="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="86" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="84" t="s">
         <v>19</v>
       </c>
@@ -9756,7 +9883,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="85"/>
       <c r="B2" s="84"/>
       <c r="C2" s="84"/>
@@ -9774,7 +9901,7 @@
       <c r="O2" s="84"/>
       <c r="P2" s="84"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="73"/>
       <c r="B3" s="72"/>
       <c r="C3" s="72"/>
@@ -9787,7 +9914,7 @@
       <c r="L3" s="72"/>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="71"/>
       <c r="B4" s="70"/>
       <c r="C4" s="70"/>
@@ -9803,7 +9930,7 @@
       <c r="L4" s="70"/>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="71"/>
       <c r="B5" s="70"/>
       <c r="C5" s="70"/>
@@ -9815,7 +9942,7 @@
       <c r="K5" s="71"/>
       <c r="L5" s="70"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="71"/>
       <c r="B6" s="70"/>
       <c r="C6" s="70"/>
@@ -9827,7 +9954,7 @@
       <c r="K6" s="71"/>
       <c r="L6" s="70"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="71"/>
       <c r="B7" s="70"/>
       <c r="C7" s="70"/>
@@ -9839,7 +9966,7 @@
       <c r="K7" s="71"/>
       <c r="L7" s="70"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="71"/>
       <c r="B8" s="70"/>
       <c r="C8" s="70"/>
@@ -9851,7 +9978,7 @@
       <c r="K8" s="71"/>
       <c r="L8" s="70"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="71"/>
       <c r="B9" s="70"/>
       <c r="C9" s="70"/>
@@ -9863,7 +9990,7 @@
       <c r="K9" s="71"/>
       <c r="L9" s="70"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="71"/>
       <c r="B10" s="70"/>
       <c r="C10" s="70"/>
@@ -9875,7 +10002,7 @@
       <c r="K10" s="71"/>
       <c r="L10" s="70"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="71"/>
       <c r="B11" s="70"/>
       <c r="C11" s="70"/>
@@ -9887,7 +10014,7 @@
       <c r="K11" s="71"/>
       <c r="L11" s="70"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="71"/>
       <c r="B12" s="70"/>
       <c r="C12" s="70"/>
@@ -9899,7 +10026,7 @@
       <c r="K12" s="71"/>
       <c r="L12" s="70"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="71"/>
       <c r="B13" s="70"/>
       <c r="C13" s="70"/>
@@ -9911,7 +10038,7 @@
       <c r="K13" s="71"/>
       <c r="L13" s="70"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -9923,7 +10050,7 @@
       <c r="K14" s="14"/>
       <c r="L14" s="13"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -9935,7 +10062,7 @@
       <c r="K15" s="14"/>
       <c r="L15" s="13"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -9947,7 +10074,7 @@
       <c r="K16" s="14"/>
       <c r="L16" s="13"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -9959,7 +10086,7 @@
       <c r="K17" s="14"/>
       <c r="L17" s="13"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -9971,7 +10098,7 @@
       <c r="K18" s="14"/>
       <c r="L18" s="13"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
@@ -9983,7 +10110,7 @@
       <c r="K19" s="14"/>
       <c r="L19" s="13"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -9995,7 +10122,7 @@
       <c r="K20" s="14"/>
       <c r="L20" s="13"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
@@ -10007,7 +10134,7 @@
       <c r="K21" s="14"/>
       <c r="L21" s="13"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -10019,7 +10146,7 @@
       <c r="K22" s="14"/>
       <c r="L22" s="13"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -10031,7 +10158,7 @@
       <c r="K23" s="14"/>
       <c r="L23" s="13"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
@@ -10043,7 +10170,7 @@
       <c r="K24" s="14"/>
       <c r="L24" s="13"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M25" s="4"/>
     </row>
   </sheetData>
@@ -10053,7 +10180,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
@@ -10064,28 +10191,28 @@
       <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="88" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.44140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="88" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" style="51" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="51" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.6640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" style="79" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.44140625" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" style="79" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.44140625" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="79" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="79" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" style="35" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3" style="35" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" style="35" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5" style="35" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" style="35" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.44140625" style="117"/>
-    <col min="17" max="16384" width="9.44140625" style="35"/>
+    <col min="16" max="16" width="9.42578125" style="117"/>
+    <col min="17" max="16384" width="9.42578125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="111" t="s">
         <v>19</v>
       </c>
@@ -10124,7 +10251,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="112" t="s">
         <v>71</v>
       </c>
@@ -10171,7 +10298,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="112" t="s">
         <v>71</v>
       </c>
@@ -10216,7 +10343,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="112" t="s">
         <v>71</v>
       </c>
@@ -10261,7 +10388,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="112" t="s">
         <v>71</v>
       </c>
@@ -10306,7 +10433,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="112" t="s">
         <v>69</v>
       </c>
@@ -10351,7 +10478,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="112" t="s">
         <v>67</v>
       </c>
@@ -10396,7 +10523,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="112" t="s">
         <v>71</v>
       </c>
@@ -10443,7 +10570,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="112" t="s">
         <v>69</v>
       </c>
@@ -10488,7 +10615,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="112" t="s">
         <v>69</v>
       </c>
@@ -10533,7 +10660,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="112" t="s">
         <v>66</v>
       </c>
@@ -10578,7 +10705,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="112" t="s">
         <v>66</v>
       </c>
@@ -10623,7 +10750,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="112" t="s">
         <v>66</v>
       </c>
@@ -10668,7 +10795,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="118" t="s">
         <v>63</v>
       </c>
@@ -10714,7 +10841,7 @@
       </c>
       <c r="P14" s="121"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="112" t="s">
         <v>63</v>
       </c>
@@ -10759,7 +10886,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="112" t="s">
         <v>63</v>
       </c>
@@ -10804,7 +10931,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="118" t="s">
         <v>63</v>
       </c>
@@ -10849,7 +10976,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="112" t="s">
         <v>84</v>
       </c>
@@ -10894,7 +11021,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="112" t="s">
         <v>83</v>
       </c>
@@ -10939,7 +11066,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="112" t="s">
         <v>83</v>
       </c>
@@ -10984,7 +11111,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="112" t="s">
         <v>83</v>
       </c>
@@ -11029,7 +11156,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="112" t="s">
         <v>84</v>
       </c>
@@ -11074,7 +11201,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="112" t="s">
         <v>72</v>
       </c>
@@ -11121,7 +11248,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="112" t="s">
         <v>71</v>
       </c>
@@ -11166,7 +11293,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="112" t="s">
         <v>72</v>
       </c>
@@ -11211,7 +11338,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="112" t="s">
         <v>72</v>
       </c>
@@ -11256,7 +11383,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="112" t="s">
         <v>97</v>
       </c>
@@ -11303,7 +11430,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="112" t="s">
         <v>71</v>
       </c>
@@ -11350,7 +11477,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="112" t="s">
         <v>77</v>
       </c>
@@ -11395,7 +11522,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="112" t="s">
         <v>89</v>
       </c>
@@ -11440,7 +11567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="112" t="s">
         <v>97</v>
       </c>
@@ -11487,7 +11614,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="112" t="s">
         <v>89</v>
       </c>
@@ -11532,7 +11659,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="112" t="s">
         <v>89</v>
       </c>
@@ -11577,7 +11704,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="112" t="s">
         <v>97</v>
       </c>
@@ -11622,7 +11749,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="112" t="s">
         <v>97</v>
       </c>
@@ -11667,7 +11794,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="112" t="s">
         <v>89</v>
       </c>
@@ -11712,7 +11839,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="112" t="s">
         <v>89</v>
       </c>
@@ -11757,7 +11884,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="112" t="s">
         <v>89</v>
       </c>
@@ -11802,7 +11929,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="112" t="s">
         <v>87</v>
       </c>
@@ -11847,7 +11974,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="112" t="s">
         <v>97</v>
       </c>
@@ -11892,7 +12019,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="112" t="s">
         <v>80</v>
       </c>
@@ -11939,7 +12066,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="112" t="s">
         <v>77</v>
       </c>
@@ -11984,7 +12111,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="112" t="s">
         <v>79</v>
       </c>
@@ -12029,7 +12156,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="112" t="s">
         <v>80</v>
       </c>
@@ -12074,7 +12201,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="112" t="s">
         <v>80</v>
       </c>
@@ -12119,7 +12246,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="112" t="s">
         <v>80</v>
       </c>
@@ -12166,7 +12293,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="112" t="s">
         <v>79</v>
       </c>
@@ -12211,7 +12338,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G48" s="115">
         <f>SUM(G2:G47)</f>
         <v>-82967225.110000014</v>
@@ -12222,8 +12349,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U1" xr:uid="{A3850EBD-1013-41F0-8978-B5269F35BB0C}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U49">
+  <autoFilter ref="A1:U1">
+    <sortState ref="A2:U49">
       <sortCondition ref="P1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
pridani vazby na ares
</commit_message>
<xml_diff>
--- a/FACTURES/doklady-CZ-06_2021-DPH.xlsx
+++ b/FACTURES/doklady-CZ-06_2021-DPH.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tkminek_local\PYTHON\XML_FILE\XML_app\FACTURES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PYTHON\PROJECTS\XML_app\XML_app\FACTURES\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF547B1-D75A-42DA-9D2A-672032A15626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6450" yWindow="1860" windowWidth="17280" windowHeight="8970" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EK 15%" sheetId="12" r:id="rId1"/>
@@ -32,12 +33,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'VK 21%'!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'VK RCH'!$A$1:$U$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="154">
   <si>
     <t>CZK</t>
   </si>
@@ -496,12 +497,15 @@
   </si>
   <si>
     <t>Ico</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
@@ -1081,8 +1085,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Čárka" xfId="1" builtinId="3"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1120,7 +1124,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1195,6 +1199,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1230,6 +1251,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1405,35 +1443,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.109375" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="74" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" style="74" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="74" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.88671875" style="74" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.109375" style="7" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5" style="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.7109375" style="7"/>
+    <col min="17" max="16384" width="10.6640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="101" t="s">
         <v>19</v>
       </c>
@@ -1475,7 +1513,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="102"/>
       <c r="B2" s="101"/>
       <c r="C2" s="101"/>
@@ -1493,7 +1531,7 @@
       <c r="O2" s="101"/>
       <c r="P2" s="101"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="102"/>
       <c r="B3" s="101"/>
       <c r="C3" s="101"/>
@@ -1511,7 +1549,7 @@
       <c r="O3" s="101"/>
       <c r="P3" s="101"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="M4" s="92" t="s">
         <v>18</v>
       </c>
@@ -1523,7 +1561,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1534,32 +1572,32 @@
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.42578125" style="64" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.44140625" style="64" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="51" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="63" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" style="63" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="64" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="99" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" style="64" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="99" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" style="64" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="65" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" style="63" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="64" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="99" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.44140625" style="64" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" style="99" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.44140625" style="64" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.109375" style="65" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2" style="65" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="65" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" style="64" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" style="65" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.44140625" style="64" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.33203125" style="36" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5" style="36" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8" style="36" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="10.28515625" style="36"/>
-    <col min="20" max="20" width="14.28515625" style="36" customWidth="1"/>
-    <col min="21" max="21" width="14.140625" style="36" customWidth="1"/>
-    <col min="22" max="16384" width="10.28515625" style="36"/>
+    <col min="18" max="19" width="10.33203125" style="36"/>
+    <col min="20" max="20" width="14.33203125" style="36" customWidth="1"/>
+    <col min="21" max="21" width="14.109375" style="36" customWidth="1"/>
+    <col min="22" max="16384" width="10.33203125" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="113" t="s">
         <v>19</v>
       </c>
@@ -1620,7 +1658,7 @@
       </c>
       <c r="W1" s="124"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="114" t="s">
         <v>58</v>
       </c>
@@ -1687,7 +1725,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="114" t="s">
         <v>79</v>
       </c>
@@ -1754,7 +1792,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>55</v>
       </c>
@@ -1822,7 +1860,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="114" t="s">
         <v>71</v>
       </c>
@@ -1889,7 +1927,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="114" t="s">
         <v>84</v>
       </c>
@@ -1956,7 +1994,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="114" t="s">
         <v>89</v>
       </c>
@@ -2023,7 +2061,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="114" t="s">
         <v>89</v>
       </c>
@@ -2090,7 +2128,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="114" t="s">
         <v>89</v>
       </c>
@@ -2157,7 +2195,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="114" t="s">
         <v>89</v>
       </c>
@@ -2224,7 +2262,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="I11" s="99">
         <f>SUM(I2:I10)</f>
         <v>-1011597.14</v>
@@ -2234,7 +2272,7 @@
         <v>-25642292.967700001</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="128" t="s">
         <v>147</v>
       </c>
@@ -2243,7 +2281,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:V10">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V10">
     <sortCondition ref="S2:S10"/>
   </sortState>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2252,7 +2290,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
@@ -2263,20 +2301,20 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.7109375" style="15"/>
+    <col min="1" max="1" width="10.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.6640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>6</v>
       </c>
@@ -2317,7 +2355,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="61" t="s">
         <v>131</v>
       </c>
@@ -2359,7 +2397,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>46</v>
       </c>
@@ -2386,7 +2424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -2399,7 +2437,7 @@
       </c>
       <c r="H4" s="22"/>
     </row>
-    <row r="5" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="21"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -2409,7 +2447,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="22"/>
     </row>
-    <row r="6" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="21"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -2419,7 +2457,7 @@
       <c r="G6" s="6"/>
       <c r="H6" s="22"/>
     </row>
-    <row r="7" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -2429,7 +2467,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="22"/>
     </row>
-    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="76" t="s">
         <v>48</v>
       </c>
@@ -2456,7 +2494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="61" t="s">
         <v>44</v>
       </c>
@@ -2483,7 +2521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="61" t="s">
         <v>39</v>
       </c>
@@ -2510,7 +2548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G11" s="92">
         <f>SUM(G8:G10)</f>
         <v>0</v>
@@ -2523,7 +2561,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2533,23 +2571,23 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="59" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="60" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.5703125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="60" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.5546875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" style="7" customWidth="1"/>
     <col min="11" max="11" width="12" style="7" customWidth="1"/>
-    <col min="12" max="16384" width="15.140625" style="7"/>
+    <col min="12" max="16384" width="15.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="67" t="s">
         <v>16</v>
       </c>
@@ -2566,7 +2604,7 @@
       <c r="J1" s="30"/>
       <c r="K1" s="32"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="33">
         <v>44348</v>
       </c>
@@ -2583,7 +2621,7 @@
       <c r="J2" s="36"/>
       <c r="K2" s="39"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>11</v>
       </c>
@@ -2600,7 +2638,7 @@
       <c r="J3" s="36"/>
       <c r="K3" s="39"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="40"/>
       <c r="B4" s="34"/>
       <c r="C4" s="35"/>
@@ -2613,7 +2651,7 @@
       <c r="J4" s="36"/>
       <c r="K4" s="39"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="s">
         <v>3</v>
       </c>
@@ -2634,7 +2672,7 @@
       </c>
       <c r="K5" s="26"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="44">
         <v>0</v>
       </c>
@@ -2663,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="44">
         <v>0.15</v>
       </c>
@@ -2692,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="44">
         <v>0.21</v>
       </c>
@@ -2721,7 +2759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="40"/>
       <c r="B9" s="47">
         <f>SUM(B7:B8)</f>
@@ -2746,7 +2784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="40"/>
       <c r="B10" s="34"/>
       <c r="C10" s="35"/>
@@ -2759,7 +2797,7 @@
       <c r="J10" s="36"/>
       <c r="K10" s="39"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="40"/>
       <c r="B11" s="34"/>
       <c r="C11" s="35"/>
@@ -2772,7 +2810,7 @@
       <c r="J11" s="36"/>
       <c r="K11" s="39"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="40"/>
       <c r="B12" s="34"/>
       <c r="C12" s="50">
@@ -2795,7 +2833,7 @@
       </c>
       <c r="K12" s="39"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="40"/>
       <c r="B13" s="34"/>
       <c r="C13" s="35"/>
@@ -2808,7 +2846,7 @@
       <c r="J13" s="36"/>
       <c r="K13" s="39"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="40"/>
       <c r="B14" s="34"/>
       <c r="C14" s="35"/>
@@ -2821,7 +2859,7 @@
       <c r="J14" s="36"/>
       <c r="K14" s="39"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="42" t="s">
         <v>2</v>
       </c>
@@ -2850,7 +2888,7 @@
         <v>1011597.14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="42" t="s">
         <v>15</v>
       </c>
@@ -2879,7 +2917,7 @@
         <v>3259367.39</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="42" t="s">
         <v>42</v>
       </c>
@@ -2908,7 +2946,7 @@
         <v>260371.04</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="42" t="s">
         <v>5</v>
       </c>
@@ -2937,7 +2975,7 @@
         <v>11285.31</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="52"/>
       <c r="B19" s="53">
         <f>SUM(B15:B18)</f>
@@ -2962,7 +3000,7 @@
         <v>4542620.88</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="74"/>
     </row>
   </sheetData>
@@ -2972,35 +3010,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.109375" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.109375" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3" style="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.33203125" style="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5" style="11" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.5703125" style="11"/>
+    <col min="17" max="16384" width="11.5546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="82" t="s">
         <v>19</v>
       </c>
@@ -3042,7 +3080,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="83"/>
       <c r="B2" s="82"/>
       <c r="C2" s="82"/>
@@ -3060,7 +3098,7 @@
       <c r="O2" s="82"/>
       <c r="P2" s="82"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="C3" s="11"/>
       <c r="E3" s="11"/>
@@ -3068,7 +3106,7 @@
       <c r="K3" s="1"/>
       <c r="M3" s="12"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="C4" s="11"/>
       <c r="E4" s="11"/>
@@ -3076,7 +3114,7 @@
       <c r="K4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="C5" s="11"/>
       <c r="E5" s="11"/>
@@ -3087,7 +3125,7 @@
       <c r="K5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="C6" s="11"/>
       <c r="E6" s="11"/>
@@ -3095,7 +3133,7 @@
       <c r="K6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="C7" s="11"/>
       <c r="E7" s="11"/>
@@ -3103,7 +3141,7 @@
       <c r="K7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="C8" s="11"/>
       <c r="E8" s="11"/>
@@ -3111,7 +3149,7 @@
       <c r="K8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="C9" s="11"/>
       <c r="E9" s="11"/>
@@ -3119,7 +3157,7 @@
       <c r="K9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="C10" s="11"/>
       <c r="E10" s="11"/>
@@ -3127,7 +3165,7 @@
       <c r="K10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="C11" s="11"/>
       <c r="E11" s="11"/>
@@ -3135,7 +3173,7 @@
       <c r="K11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="C12" s="11"/>
       <c r="E12" s="11"/>
@@ -3143,7 +3181,7 @@
       <c r="K12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="C13" s="11"/>
       <c r="E13" s="11"/>
@@ -3151,7 +3189,7 @@
       <c r="K13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="C14" s="11"/>
       <c r="E14" s="11"/>
@@ -3159,7 +3197,7 @@
       <c r="K14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="C15" s="11"/>
       <c r="E15" s="11"/>
@@ -3167,7 +3205,7 @@
       <c r="K15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="C16" s="11"/>
       <c r="E16" s="11"/>
@@ -3175,7 +3213,7 @@
       <c r="K16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="C17" s="11"/>
       <c r="E17" s="11"/>
@@ -3183,7 +3221,7 @@
       <c r="K17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="C18" s="11"/>
       <c r="E18" s="11"/>
@@ -3191,7 +3229,7 @@
       <c r="K18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="C19" s="11"/>
       <c r="E19" s="11"/>
@@ -3199,7 +3237,7 @@
       <c r="K19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="C20" s="11"/>
       <c r="E20" s="11"/>
@@ -3207,7 +3245,7 @@
       <c r="K20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="C21" s="11"/>
       <c r="E21" s="11"/>
@@ -3215,7 +3253,7 @@
       <c r="K21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="C22" s="11"/>
       <c r="E22" s="11"/>
@@ -3223,7 +3261,7 @@
       <c r="K22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="C23" s="11"/>
       <c r="E23" s="11"/>
@@ -3231,7 +3269,7 @@
       <c r="K23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="C24" s="11"/>
       <c r="E24" s="11"/>
@@ -3239,7 +3277,7 @@
       <c r="K24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="C25" s="11"/>
       <c r="E25" s="11"/>
@@ -3247,7 +3285,7 @@
       <c r="K25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="C26" s="11"/>
       <c r="E26" s="11"/>
@@ -3255,7 +3293,7 @@
       <c r="K26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="C27" s="11"/>
       <c r="E27" s="11"/>
@@ -3263,7 +3301,7 @@
       <c r="K27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="C28" s="11"/>
       <c r="E28" s="11"/>
@@ -3271,7 +3309,7 @@
       <c r="K28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="C29" s="11"/>
       <c r="E29" s="11"/>
@@ -3279,7 +3317,7 @@
       <c r="K29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="C30" s="11"/>
       <c r="E30" s="11"/>
@@ -3287,7 +3325,7 @@
       <c r="K30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="C31" s="11"/>
       <c r="E31" s="11"/>
@@ -3295,7 +3333,7 @@
       <c r="K31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="C32" s="11"/>
       <c r="E32" s="11"/>
@@ -3303,7 +3341,7 @@
       <c r="K32" s="1"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="C33" s="11"/>
       <c r="E33" s="11"/>
@@ -3311,7 +3349,7 @@
       <c r="K33" s="1"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="C34" s="11"/>
       <c r="E34" s="11"/>
@@ -3319,7 +3357,7 @@
       <c r="K34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="C35" s="11"/>
       <c r="E35" s="11"/>
@@ -3327,7 +3365,7 @@
       <c r="K35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="C36" s="11"/>
       <c r="E36" s="11"/>
@@ -3335,7 +3373,7 @@
       <c r="K36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="C37" s="11"/>
       <c r="E37" s="11"/>
@@ -3343,7 +3381,7 @@
       <c r="K37" s="1"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="C38" s="11"/>
       <c r="E38" s="11"/>
@@ -3351,7 +3389,7 @@
       <c r="K38" s="1"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="C39" s="11"/>
       <c r="E39" s="11"/>
@@ -3359,7 +3397,7 @@
       <c r="K39" s="1"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="C40" s="11"/>
       <c r="E40" s="11"/>
@@ -3367,7 +3405,7 @@
       <c r="K40" s="1"/>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="C41" s="11"/>
       <c r="E41" s="11"/>
@@ -3375,7 +3413,7 @@
       <c r="K41" s="1"/>
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="C42" s="11"/>
       <c r="E42" s="11"/>
@@ -3383,7 +3421,7 @@
       <c r="K42" s="1"/>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="C43" s="11"/>
       <c r="E43" s="11"/>
@@ -3391,7 +3429,7 @@
       <c r="K43" s="1"/>
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="C44" s="11"/>
       <c r="E44" s="11"/>
@@ -3399,7 +3437,7 @@
       <c r="K44" s="1"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="C45" s="11"/>
       <c r="E45" s="11"/>
@@ -3407,7 +3445,7 @@
       <c r="K45" s="1"/>
       <c r="M45" s="1"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="C46" s="11"/>
       <c r="E46" s="11"/>
@@ -3415,7 +3453,7 @@
       <c r="K46" s="1"/>
       <c r="M46" s="1"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="C47" s="11"/>
       <c r="E47" s="11"/>
@@ -3423,7 +3461,7 @@
       <c r="K47" s="1"/>
       <c r="M47" s="1"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="C48" s="11"/>
       <c r="E48" s="11"/>
@@ -3431,7 +3469,7 @@
       <c r="K48" s="1"/>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="C49" s="11"/>
       <c r="E49" s="11"/>
@@ -3439,7 +3477,7 @@
       <c r="K49" s="1"/>
       <c r="M49" s="1"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="C50" s="11"/>
       <c r="E50" s="11"/>
@@ -3447,7 +3485,7 @@
       <c r="K50" s="1"/>
       <c r="M50" s="1"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="C51" s="11"/>
       <c r="E51" s="11"/>
@@ -3455,7 +3493,7 @@
       <c r="K51" s="1"/>
       <c r="M51" s="1"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="C52" s="11"/>
       <c r="E52" s="11"/>
@@ -3463,7 +3501,7 @@
       <c r="K52" s="1"/>
       <c r="M52" s="1"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="C53" s="11"/>
       <c r="E53" s="11"/>
@@ -3471,7 +3509,7 @@
       <c r="K53" s="1"/>
       <c r="M53" s="1"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="C54" s="11"/>
       <c r="E54" s="11"/>
@@ -3479,7 +3517,7 @@
       <c r="K54" s="1"/>
       <c r="M54" s="1"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="C55" s="11"/>
       <c r="E55" s="11"/>
@@ -3487,7 +3525,7 @@
       <c r="K55" s="1"/>
       <c r="M55" s="1"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="C56" s="11"/>
       <c r="E56" s="11"/>
@@ -3495,7 +3533,7 @@
       <c r="K56" s="1"/>
       <c r="M56" s="1"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="C57" s="11"/>
       <c r="E57" s="11"/>
@@ -3503,7 +3541,7 @@
       <c r="K57" s="1"/>
       <c r="M57" s="1"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="C58" s="11"/>
       <c r="E58" s="11"/>
@@ -3511,7 +3549,7 @@
       <c r="K58" s="1"/>
       <c r="M58" s="1"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="C59" s="11"/>
       <c r="E59" s="11"/>
@@ -3519,7 +3557,7 @@
       <c r="K59" s="1"/>
       <c r="M59" s="1"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="C60" s="11"/>
       <c r="E60" s="11"/>
@@ -3527,7 +3565,7 @@
       <c r="K60" s="1"/>
       <c r="M60" s="1"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="C61" s="11"/>
       <c r="E61" s="11"/>
@@ -3535,7 +3573,7 @@
       <c r="K61" s="1"/>
       <c r="M61" s="1"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="C62" s="11"/>
       <c r="E62" s="11"/>
@@ -3543,7 +3581,7 @@
       <c r="K62" s="1"/>
       <c r="M62" s="1"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="C63" s="11"/>
       <c r="E63" s="11"/>
@@ -3551,7 +3589,7 @@
       <c r="K63" s="1"/>
       <c r="M63" s="1"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="C64" s="11"/>
       <c r="E64" s="11"/>
@@ -3559,7 +3597,7 @@
       <c r="K64" s="1"/>
       <c r="M64" s="1"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="C65" s="11"/>
       <c r="E65" s="11"/>
@@ -3567,7 +3605,7 @@
       <c r="K65" s="1"/>
       <c r="M65" s="1"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="C66" s="11"/>
       <c r="E66" s="11"/>
@@ -3575,7 +3613,7 @@
       <c r="K66" s="1"/>
       <c r="M66" s="1"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="C67" s="11"/>
       <c r="E67" s="11"/>
@@ -3583,7 +3621,7 @@
       <c r="K67" s="1"/>
       <c r="M67" s="1"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="C68" s="11"/>
       <c r="E68" s="11"/>
@@ -3591,7 +3629,7 @@
       <c r="K68" s="1"/>
       <c r="M68" s="1"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="C69" s="11"/>
       <c r="E69" s="11"/>
@@ -3599,7 +3637,7 @@
       <c r="K69" s="1"/>
       <c r="M69" s="1"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="C70" s="11"/>
       <c r="E70" s="11"/>
@@ -3607,7 +3645,7 @@
       <c r="K70" s="1"/>
       <c r="M70" s="1"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="C71" s="11"/>
       <c r="E71" s="11"/>
@@ -3615,7 +3653,7 @@
       <c r="K71" s="1"/>
       <c r="M71" s="1"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="C72" s="11"/>
       <c r="E72" s="11"/>
@@ -3623,7 +3661,7 @@
       <c r="K72" s="1"/>
       <c r="M72" s="1"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="C73" s="11"/>
       <c r="E73" s="11"/>
@@ -3631,7 +3669,7 @@
       <c r="K73" s="1"/>
       <c r="M73" s="1"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="C74" s="11"/>
       <c r="E74" s="11"/>
@@ -3639,7 +3677,7 @@
       <c r="K74" s="1"/>
       <c r="M74" s="1"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="C75" s="11"/>
       <c r="E75" s="11"/>
@@ -3647,7 +3685,7 @@
       <c r="K75" s="1"/>
       <c r="M75" s="1"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="C76" s="11"/>
       <c r="E76" s="11"/>
@@ -3655,7 +3693,7 @@
       <c r="K76" s="1"/>
       <c r="M76" s="1"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="C77" s="11"/>
       <c r="E77" s="11"/>
@@ -3663,7 +3701,7 @@
       <c r="K77" s="1"/>
       <c r="M77" s="1"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="C78" s="11"/>
       <c r="E78" s="11"/>
@@ -3671,7 +3709,7 @@
       <c r="K78" s="1"/>
       <c r="M78" s="1"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="C79" s="11"/>
       <c r="E79" s="11"/>
@@ -3679,7 +3717,7 @@
       <c r="K79" s="1"/>
       <c r="M79" s="1"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="C80" s="11"/>
       <c r="E80" s="11"/>
@@ -3687,7 +3725,7 @@
       <c r="K80" s="1"/>
       <c r="M80" s="1"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="C81" s="11"/>
       <c r="E81" s="11"/>
@@ -3695,7 +3733,7 @@
       <c r="K81" s="1"/>
       <c r="M81" s="1"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="C82" s="11"/>
       <c r="E82" s="11"/>
@@ -3703,7 +3741,7 @@
       <c r="K82" s="1"/>
       <c r="M82" s="1"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="C83" s="11"/>
       <c r="E83" s="11"/>
@@ -3718,35 +3756,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr filterMode="1">
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P70"/>
+  <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="T53" sqref="T53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="90" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.140625" style="51" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="51" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="51" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" style="63" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="79" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="79" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" style="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" style="90" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5546875" style="63" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="79" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.44140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="79" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.44140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" style="35" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3" style="35" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="11.5703125" style="35"/>
+    <col min="13" max="16384" width="11.5546875" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="105" t="s">
         <v>19</v>
       </c>
@@ -3788,7 +3826,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="129" t="s">
         <v>55</v>
       </c>
@@ -3835,7 +3873,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="129" t="s">
         <v>58</v>
       </c>
@@ -3882,7 +3920,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="129" t="s">
         <v>55</v>
       </c>
@@ -3929,7 +3967,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="129" t="s">
         <v>55</v>
       </c>
@@ -3976,7 +4014,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="129" t="s">
         <v>55</v>
       </c>
@@ -4022,8 +4060,11 @@
       <c r="O6" s="130">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R6" s="132" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="129" t="s">
         <v>55</v>
       </c>
@@ -4070,7 +4111,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="129" t="s">
         <v>55</v>
       </c>
@@ -4117,7 +4158,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="129" t="s">
         <v>57</v>
       </c>
@@ -4164,7 +4205,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="129" t="s">
         <v>58</v>
       </c>
@@ -4211,7 +4252,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="129" t="s">
         <v>61</v>
       </c>
@@ -4258,7 +4299,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="129" t="s">
         <v>67</v>
       </c>
@@ -4305,7 +4346,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="129" t="s">
         <v>69</v>
       </c>
@@ -4352,7 +4393,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="129" t="s">
         <v>69</v>
       </c>
@@ -4399,7 +4440,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="133" t="s">
         <v>57</v>
       </c>
@@ -4446,10 +4487,10 @@
         <v>12</v>
       </c>
       <c r="P15" s="132">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27830322</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="133" t="s">
         <v>57</v>
       </c>
@@ -4496,10 +4537,10 @@
         <v>12</v>
       </c>
       <c r="P16" s="132">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27830322</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="133" t="s">
         <v>58</v>
       </c>
@@ -4546,10 +4587,10 @@
         <v>12</v>
       </c>
       <c r="P17" s="132">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27830322</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="133" t="s">
         <v>58</v>
       </c>
@@ -4596,10 +4637,10 @@
         <v>12</v>
       </c>
       <c r="P18" s="132">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27830322</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="133" t="s">
         <v>61</v>
       </c>
@@ -4646,10 +4687,10 @@
         <v>12</v>
       </c>
       <c r="P19" s="132">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27830322</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="133" t="s">
         <v>61</v>
       </c>
@@ -4696,10 +4737,10 @@
         <v>12</v>
       </c>
       <c r="P20" s="132">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27830322</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="133" t="s">
         <v>63</v>
       </c>
@@ -4746,10 +4787,10 @@
         <v>12</v>
       </c>
       <c r="P21" s="132">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27830322</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="133" t="s">
         <v>63</v>
       </c>
@@ -4796,10 +4837,10 @@
         <v>12</v>
       </c>
       <c r="P22" s="132">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27830322</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="133" t="s">
         <v>66</v>
       </c>
@@ -4846,10 +4887,10 @@
         <v>12</v>
       </c>
       <c r="P23" s="132">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27830322</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="133" t="s">
         <v>67</v>
       </c>
@@ -4896,10 +4937,10 @@
         <v>12</v>
       </c>
       <c r="P24" s="132">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27830322</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="133" t="s">
         <v>67</v>
       </c>
@@ -4946,10 +4987,10 @@
         <v>12</v>
       </c>
       <c r="P25" s="132">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27830322</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="133" t="s">
         <v>67</v>
       </c>
@@ -4996,10 +5037,10 @@
         <v>12</v>
       </c>
       <c r="P26" s="132">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27830322</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="133" t="s">
         <v>69</v>
       </c>
@@ -5046,10 +5087,10 @@
         <v>12</v>
       </c>
       <c r="P27" s="132">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27830322</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="133" t="s">
         <v>69</v>
       </c>
@@ -5096,10 +5137,10 @@
         <v>12</v>
       </c>
       <c r="P28" s="132">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27830322</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="133" t="s">
         <v>71</v>
       </c>
@@ -5146,10 +5187,10 @@
         <v>12</v>
       </c>
       <c r="P29" s="132">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27830322</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" s="132" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="133" t="s">
         <v>71</v>
       </c>
@@ -5196,10 +5237,10 @@
         <v>12</v>
       </c>
       <c r="P30" s="132">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+        <v>27830322</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="106" t="s">
         <v>72</v>
       </c>
@@ -5246,10 +5287,10 @@
         <v>12</v>
       </c>
       <c r="P31" s="132">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+        <v>27830322</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="106" t="s">
         <v>72</v>
       </c>
@@ -5295,11 +5336,11 @@
       <c r="O32" s="105">
         <v>12</v>
       </c>
-      <c r="P32" s="132">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P32">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="106" t="s">
         <v>72</v>
       </c>
@@ -5345,11 +5386,11 @@
       <c r="O33" s="105">
         <v>12</v>
       </c>
-      <c r="P33" s="132">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P33" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="106" t="s">
         <v>72</v>
       </c>
@@ -5395,11 +5436,11 @@
       <c r="O34" s="105">
         <v>12</v>
       </c>
-      <c r="P34" s="132">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P34" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="106" t="s">
         <v>75</v>
       </c>
@@ -5445,11 +5486,11 @@
       <c r="O35" s="105">
         <v>12</v>
       </c>
-      <c r="P35" s="132">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P35" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="106" t="s">
         <v>75</v>
       </c>
@@ -5495,11 +5536,11 @@
       <c r="O36" s="105">
         <v>12</v>
       </c>
-      <c r="P36" s="132">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P36" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="106" t="s">
         <v>75</v>
       </c>
@@ -5545,11 +5586,11 @@
       <c r="O37" s="105">
         <v>12</v>
       </c>
-      <c r="P37" s="132">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P37" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="106" t="s">
         <v>75</v>
       </c>
@@ -5595,11 +5636,11 @@
       <c r="O38" s="105">
         <v>12</v>
       </c>
-      <c r="P38" s="132">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P38" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="106" t="s">
         <v>75</v>
       </c>
@@ -5645,11 +5686,11 @@
       <c r="O39" s="105">
         <v>12</v>
       </c>
-      <c r="P39" s="132">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P39" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="106" t="s">
         <v>77</v>
       </c>
@@ -5695,11 +5736,11 @@
       <c r="O40" s="105">
         <v>12</v>
       </c>
-      <c r="P40" s="132">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P40" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="114" t="s">
         <v>78</v>
       </c>
@@ -5745,11 +5786,11 @@
       <c r="O41" s="113">
         <v>12</v>
       </c>
-      <c r="P41" s="132">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P41" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="114" t="s">
         <v>79</v>
       </c>
@@ -5795,11 +5836,11 @@
       <c r="O42" s="113">
         <v>12</v>
       </c>
-      <c r="P42" s="132">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P42" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="114" t="s">
         <v>79</v>
       </c>
@@ -5845,11 +5886,11 @@
       <c r="O43" s="113">
         <v>12</v>
       </c>
-      <c r="P43" s="132">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P43" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="114" t="s">
         <v>79</v>
       </c>
@@ -5895,11 +5936,11 @@
       <c r="O44" s="113">
         <v>12</v>
       </c>
-      <c r="P44" s="132">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P44" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="114" t="s">
         <v>79</v>
       </c>
@@ -5945,11 +5986,11 @@
       <c r="O45" s="113">
         <v>12</v>
       </c>
-      <c r="P45" s="132">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P45" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="114" t="s">
         <v>80</v>
       </c>
@@ -5995,11 +6036,11 @@
       <c r="O46" s="113">
         <v>12</v>
       </c>
-      <c r="P46" s="132">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P46" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="114" t="s">
         <v>80</v>
       </c>
@@ -6045,11 +6086,11 @@
       <c r="O47" s="113">
         <v>12</v>
       </c>
-      <c r="P47" s="132">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P47" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="114" t="s">
         <v>81</v>
       </c>
@@ -6095,11 +6136,11 @@
       <c r="O48" s="113">
         <v>12</v>
       </c>
-      <c r="P48" s="132">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P48" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="114" t="s">
         <v>81</v>
       </c>
@@ -6145,11 +6186,11 @@
       <c r="O49" s="113">
         <v>12</v>
       </c>
-      <c r="P49" s="132">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P49" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="114" t="s">
         <v>83</v>
       </c>
@@ -6195,11 +6236,11 @@
       <c r="O50" s="113">
         <v>12</v>
       </c>
-      <c r="P50" s="132">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P50" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="114" t="s">
         <v>83</v>
       </c>
@@ -6245,11 +6286,11 @@
       <c r="O51" s="113">
         <v>12</v>
       </c>
-      <c r="P51" s="132">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P51" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="114" t="s">
         <v>84</v>
       </c>
@@ -6295,11 +6336,11 @@
       <c r="O52" s="113">
         <v>12</v>
       </c>
-      <c r="P52" s="132">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P52" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="114" t="s">
         <v>84</v>
       </c>
@@ -6345,11 +6386,11 @@
       <c r="O53" s="113">
         <v>12</v>
       </c>
-      <c r="P53" s="132">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P53" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="114" t="s">
         <v>84</v>
       </c>
@@ -6395,11 +6436,11 @@
       <c r="O54" s="113">
         <v>12</v>
       </c>
-      <c r="P54" s="132">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P54" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="114" t="s">
         <v>84</v>
       </c>
@@ -6445,11 +6486,11 @@
       <c r="O55" s="113">
         <v>12</v>
       </c>
-      <c r="P55" s="132">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P55" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="114" t="s">
         <v>84</v>
       </c>
@@ -6495,11 +6536,11 @@
       <c r="O56" s="113">
         <v>12</v>
       </c>
-      <c r="P56" s="132">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P56" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="114" t="s">
         <v>84</v>
       </c>
@@ -6545,11 +6586,11 @@
       <c r="O57" s="113">
         <v>12</v>
       </c>
-      <c r="P57" s="132">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P57" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" s="114" t="s">
         <v>87</v>
       </c>
@@ -6595,11 +6636,11 @@
       <c r="O58" s="113">
         <v>12</v>
       </c>
-      <c r="P58" s="132">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P58" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="114" t="s">
         <v>87</v>
       </c>
@@ -6645,11 +6686,11 @@
       <c r="O59" s="113">
         <v>12</v>
       </c>
-      <c r="P59" s="132">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P59" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" s="114" t="s">
         <v>87</v>
       </c>
@@ -6695,11 +6736,11 @@
       <c r="O60" s="113">
         <v>12</v>
       </c>
-      <c r="P60" s="132">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P60" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="114" t="s">
         <v>87</v>
       </c>
@@ -6745,11 +6786,11 @@
       <c r="O61" s="113">
         <v>12</v>
       </c>
-      <c r="P61" s="132">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P61" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" s="114" t="s">
         <v>89</v>
       </c>
@@ -6795,11 +6836,11 @@
       <c r="O62" s="113">
         <v>12</v>
       </c>
-      <c r="P62" s="132">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P62" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="114" t="s">
         <v>89</v>
       </c>
@@ -6845,11 +6886,11 @@
       <c r="O63" s="113">
         <v>12</v>
       </c>
-      <c r="P63" s="132">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P63" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" s="114" t="s">
         <v>89</v>
       </c>
@@ -6895,11 +6936,11 @@
       <c r="O64" s="113">
         <v>12</v>
       </c>
-      <c r="P64" s="132">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P64" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="114" t="s">
         <v>89</v>
       </c>
@@ -6945,11 +6986,11 @@
       <c r="O65" s="113">
         <v>12</v>
       </c>
-      <c r="P65" s="132">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P65" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="114" t="s">
         <v>89</v>
       </c>
@@ -6995,11 +7036,11 @@
       <c r="O66" s="113">
         <v>12</v>
       </c>
-      <c r="P66" s="132">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P66" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" s="114" t="s">
         <v>89</v>
       </c>
@@ -7045,11 +7086,11 @@
       <c r="O67" s="113">
         <v>12</v>
       </c>
-      <c r="P67" s="132">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P67" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" s="114" t="s">
         <v>89</v>
       </c>
@@ -7095,11 +7136,11 @@
       <c r="O68" s="113">
         <v>12</v>
       </c>
-      <c r="P68" s="132">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P68" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" s="114" t="s">
         <v>89</v>
       </c>
@@ -7145,23 +7186,23 @@
       <c r="O69" s="113">
         <v>12</v>
       </c>
-      <c r="P69" s="132">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P69" s="113">
+        <v>18107184</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G70" s="115">
         <f>SUM(G15:G69)</f>
         <v>39745164.280000009</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:O70">
+  <autoFilter ref="A2:O70" xr:uid="{00000000-0009-0000-0000-000002000000}">
     <filterColumn colId="14">
       <colorFilter dxfId="1" cellColor="0"/>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A2:O69">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O69">
     <sortCondition sortBy="cellColor" ref="O69" dxfId="0"/>
   </sortState>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -7170,7 +7211,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
@@ -7181,29 +7222,29 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="89" customWidth="1"/>
-    <col min="2" max="2" width="3.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" style="89" customWidth="1"/>
+    <col min="2" max="2" width="3.109375" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="51" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="51" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="51" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" style="63" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="64" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="100" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" style="100" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="64" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" style="64" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="64" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="64" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="100" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.44140625" style="100" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="64" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.44140625" style="64" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.109375" style="64" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2" style="64" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="65" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" style="64" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" style="65" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" style="64" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.33203125" style="36" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5" style="36" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8" style="36" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="11.140625" style="36"/>
+    <col min="18" max="16384" width="11.109375" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="103" t="s">
         <v>19</v>
       </c>
@@ -7264,7 +7305,7 @@
       </c>
       <c r="W1" s="124"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="108" t="s">
         <v>58</v>
       </c>
@@ -7333,7 +7374,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="108" t="s">
         <v>75</v>
       </c>
@@ -7402,7 +7443,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="108" t="s">
         <v>75</v>
       </c>
@@ -7471,7 +7512,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="108" t="s">
         <v>78</v>
       </c>
@@ -7540,7 +7581,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="108" t="s">
         <v>78</v>
       </c>
@@ -7609,7 +7650,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="108" t="s">
         <v>78</v>
       </c>
@@ -7678,7 +7719,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="108" t="s">
         <v>78</v>
       </c>
@@ -7747,7 +7788,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="108" t="s">
         <v>78</v>
       </c>
@@ -7816,7 +7857,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="108" t="s">
         <v>97</v>
       </c>
@@ -7885,7 +7926,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="108" t="s">
         <v>97</v>
       </c>
@@ -7954,7 +7995,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="I12" s="64">
         <f>SUM(I2:I11)</f>
         <v>1263840.33</v>
@@ -7971,7 +8012,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -7981,16 +8022,16 @@
       <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="113" t="s">
         <v>19</v>
       </c>
@@ -8050,7 +8091,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="114" t="s">
         <v>58</v>
       </c>
@@ -8119,7 +8160,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="114" t="s">
         <v>78</v>
       </c>
@@ -8188,7 +8229,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="114" t="s">
         <v>97</v>
       </c>
@@ -8257,7 +8298,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="114"/>
       <c r="C5" s="91"/>
       <c r="D5" s="91"/>
@@ -8279,7 +8320,7 @@
       <c r="U5" s="36"/>
       <c r="V5" s="36"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="114" t="s">
         <v>75</v>
       </c>
@@ -8348,7 +8389,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="114" t="s">
         <v>75</v>
       </c>
@@ -8417,7 +8458,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="114" t="s">
         <v>78</v>
       </c>
@@ -8486,7 +8527,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="114" t="s">
         <v>78</v>
       </c>
@@ -8555,7 +8596,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="114" t="s">
         <v>78</v>
       </c>
@@ -8624,7 +8665,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="114" t="s">
         <v>78</v>
       </c>
@@ -8693,7 +8734,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="114" t="s">
         <v>97</v>
       </c>
@@ -8762,7 +8803,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="89"/>
       <c r="B13" s="36"/>
       <c r="C13" s="51"/>
@@ -8795,12 +8836,12 @@
       <c r="U13" s="36"/>
       <c r="V13" s="36"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="113" t="s">
         <v>19</v>
       </c>
@@ -8860,7 +8901,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="114" t="s">
         <v>58</v>
       </c>
@@ -8927,7 +8968,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="114" t="s">
         <v>79</v>
       </c>
@@ -8994,7 +9035,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="23" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="114"/>
       <c r="G23" s="114"/>
       <c r="I23" s="114"/>
@@ -9013,7 +9054,7 @@
       <c r="U23" s="36"/>
       <c r="V23" s="36"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>55</v>
       </c>
@@ -9081,7 +9122,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="126"/>
       <c r="C25" s="126"/>
@@ -9107,7 +9148,7 @@
       <c r="U25" s="36"/>
       <c r="V25" s="36"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="114" t="s">
         <v>71</v>
       </c>
@@ -9174,7 +9215,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="114" t="s">
         <v>84</v>
       </c>
@@ -9241,7 +9282,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="114" t="s">
         <v>89</v>
       </c>
@@ -9308,7 +9349,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="114"/>
       <c r="G29" s="114"/>
       <c r="I29" s="114"/>
@@ -9327,7 +9368,7 @@
       <c r="U29" s="36"/>
       <c r="V29" s="36"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="114" t="s">
         <v>89</v>
       </c>
@@ -9394,7 +9435,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" s="113" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="114"/>
       <c r="G31" s="114"/>
       <c r="I31" s="114"/>
@@ -9410,7 +9451,7 @@
       <c r="U31" s="36"/>
       <c r="V31" s="36"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="114" t="s">
         <v>89</v>
       </c>
@@ -9477,7 +9518,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" s="114" t="s">
         <v>89</v>
       </c>
@@ -9544,7 +9585,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="36"/>
       <c r="B34" s="64"/>
       <c r="C34" s="51"/>
@@ -9577,7 +9618,7 @@
       <c r="U34" s="36"/>
       <c r="V34" s="36"/>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" s="128" t="s">
         <v>147</v>
       </c>
@@ -9606,7 +9647,7 @@
       <c r="V35" s="36"/>
     </row>
   </sheetData>
-  <sortState ref="A3:V12">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:V12">
     <sortCondition ref="S3:S12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -9615,7 +9656,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
@@ -9626,25 +9667,25 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="114" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="114" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="80" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="114" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="114" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.109375" style="80" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2" style="80" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="109" t="s">
         <v>19</v>
       </c>
@@ -9683,7 +9724,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="110" t="s">
         <v>55</v>
       </c>
@@ -9735,35 +9776,35 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.44140625" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.109375" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5" style="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.140625" style="7"/>
+    <col min="17" max="16384" width="11.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="97" t="s">
         <v>19</v>
       </c>
@@ -9805,7 +9846,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F5" s="92" t="s">
         <v>18</v>
       </c>
@@ -9817,31 +9858,31 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="86" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="86" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="86" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.109375" style="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3" style="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="86" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="84" t="s">
         <v>19</v>
       </c>
@@ -9883,7 +9924,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="85"/>
       <c r="B2" s="84"/>
       <c r="C2" s="84"/>
@@ -9901,7 +9942,7 @@
       <c r="O2" s="84"/>
       <c r="P2" s="84"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="73"/>
       <c r="B3" s="72"/>
       <c r="C3" s="72"/>
@@ -9914,7 +9955,7 @@
       <c r="L3" s="72"/>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="71"/>
       <c r="B4" s="70"/>
       <c r="C4" s="70"/>
@@ -9930,7 +9971,7 @@
       <c r="L4" s="70"/>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="71"/>
       <c r="B5" s="70"/>
       <c r="C5" s="70"/>
@@ -9942,7 +9983,7 @@
       <c r="K5" s="71"/>
       <c r="L5" s="70"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="71"/>
       <c r="B6" s="70"/>
       <c r="C6" s="70"/>
@@ -9954,7 +9995,7 @@
       <c r="K6" s="71"/>
       <c r="L6" s="70"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="71"/>
       <c r="B7" s="70"/>
       <c r="C7" s="70"/>
@@ -9966,7 +10007,7 @@
       <c r="K7" s="71"/>
       <c r="L7" s="70"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="71"/>
       <c r="B8" s="70"/>
       <c r="C8" s="70"/>
@@ -9978,7 +10019,7 @@
       <c r="K8" s="71"/>
       <c r="L8" s="70"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="71"/>
       <c r="B9" s="70"/>
       <c r="C9" s="70"/>
@@ -9990,7 +10031,7 @@
       <c r="K9" s="71"/>
       <c r="L9" s="70"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="71"/>
       <c r="B10" s="70"/>
       <c r="C10" s="70"/>
@@ -10002,7 +10043,7 @@
       <c r="K10" s="71"/>
       <c r="L10" s="70"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="71"/>
       <c r="B11" s="70"/>
       <c r="C11" s="70"/>
@@ -10014,7 +10055,7 @@
       <c r="K11" s="71"/>
       <c r="L11" s="70"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="71"/>
       <c r="B12" s="70"/>
       <c r="C12" s="70"/>
@@ -10026,7 +10067,7 @@
       <c r="K12" s="71"/>
       <c r="L12" s="70"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="71"/>
       <c r="B13" s="70"/>
       <c r="C13" s="70"/>
@@ -10038,7 +10079,7 @@
       <c r="K13" s="71"/>
       <c r="L13" s="70"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -10050,7 +10091,7 @@
       <c r="K14" s="14"/>
       <c r="L14" s="13"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -10062,7 +10103,7 @@
       <c r="K15" s="14"/>
       <c r="L15" s="13"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -10074,7 +10115,7 @@
       <c r="K16" s="14"/>
       <c r="L16" s="13"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -10086,7 +10127,7 @@
       <c r="K17" s="14"/>
       <c r="L17" s="13"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -10098,7 +10139,7 @@
       <c r="K18" s="14"/>
       <c r="L18" s="13"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
@@ -10110,7 +10151,7 @@
       <c r="K19" s="14"/>
       <c r="L19" s="13"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -10122,7 +10163,7 @@
       <c r="K20" s="14"/>
       <c r="L20" s="13"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
@@ -10134,7 +10175,7 @@
       <c r="K21" s="14"/>
       <c r="L21" s="13"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -10146,7 +10187,7 @@
       <c r="K22" s="14"/>
       <c r="L22" s="13"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -10158,7 +10199,7 @@
       <c r="K23" s="14"/>
       <c r="L23" s="13"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
@@ -10170,7 +10211,7 @@
       <c r="K24" s="14"/>
       <c r="L24" s="13"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M25" s="4"/>
     </row>
   </sheetData>
@@ -10180,7 +10221,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
@@ -10191,28 +10232,28 @@
       <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="88" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.42578125" style="51" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" style="88" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.44140625" style="51" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="51" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="51" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="79" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="79" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.6640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="79" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.44140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" style="79" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.44140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.109375" style="35" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3" style="35" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.28515625" style="35" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.33203125" style="35" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5" style="35" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" style="35" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.42578125" style="117"/>
-    <col min="17" max="16384" width="9.42578125" style="35"/>
+    <col min="16" max="16" width="9.44140625" style="117"/>
+    <col min="17" max="16384" width="9.44140625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="111" t="s">
         <v>19</v>
       </c>
@@ -10251,7 +10292,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="112" t="s">
         <v>71</v>
       </c>
@@ -10298,7 +10339,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="112" t="s">
         <v>71</v>
       </c>
@@ -10343,7 +10384,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="112" t="s">
         <v>71</v>
       </c>
@@ -10388,7 +10429,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="112" t="s">
         <v>71</v>
       </c>
@@ -10433,7 +10474,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="112" t="s">
         <v>69</v>
       </c>
@@ -10478,7 +10519,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="112" t="s">
         <v>67</v>
       </c>
@@ -10523,7 +10564,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="112" t="s">
         <v>71</v>
       </c>
@@ -10570,7 +10611,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="112" t="s">
         <v>69</v>
       </c>
@@ -10615,7 +10656,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="112" t="s">
         <v>69</v>
       </c>
@@ -10660,7 +10701,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="112" t="s">
         <v>66</v>
       </c>
@@ -10705,7 +10746,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="112" t="s">
         <v>66</v>
       </c>
@@ -10750,7 +10791,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="112" t="s">
         <v>66</v>
       </c>
@@ -10795,7 +10836,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="118" t="s">
         <v>63</v>
       </c>
@@ -10841,7 +10882,7 @@
       </c>
       <c r="P14" s="121"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="112" t="s">
         <v>63</v>
       </c>
@@ -10886,7 +10927,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="112" t="s">
         <v>63</v>
       </c>
@@ -10931,7 +10972,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="118" t="s">
         <v>63</v>
       </c>
@@ -10976,7 +11017,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="112" t="s">
         <v>84</v>
       </c>
@@ -11021,7 +11062,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="112" t="s">
         <v>83</v>
       </c>
@@ -11066,7 +11107,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="112" t="s">
         <v>83</v>
       </c>
@@ -11111,7 +11152,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="112" t="s">
         <v>83</v>
       </c>
@@ -11156,7 +11197,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="112" t="s">
         <v>84</v>
       </c>
@@ -11201,7 +11242,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="112" t="s">
         <v>72</v>
       </c>
@@ -11248,7 +11289,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="112" t="s">
         <v>71</v>
       </c>
@@ -11293,7 +11334,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="112" t="s">
         <v>72</v>
       </c>
@@ -11338,7 +11379,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="112" t="s">
         <v>72</v>
       </c>
@@ -11383,7 +11424,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="112" t="s">
         <v>97</v>
       </c>
@@ -11430,7 +11471,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="112" t="s">
         <v>71</v>
       </c>
@@ -11477,7 +11518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="112" t="s">
         <v>77</v>
       </c>
@@ -11522,7 +11563,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="112" t="s">
         <v>89</v>
       </c>
@@ -11567,7 +11608,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="112" t="s">
         <v>97</v>
       </c>
@@ -11614,7 +11655,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="112" t="s">
         <v>89</v>
       </c>
@@ -11659,7 +11700,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="112" t="s">
         <v>89</v>
       </c>
@@ -11704,7 +11745,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="112" t="s">
         <v>97</v>
       </c>
@@ -11749,7 +11790,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="112" t="s">
         <v>97</v>
       </c>
@@ -11794,7 +11835,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="112" t="s">
         <v>89</v>
       </c>
@@ -11839,7 +11880,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="112" t="s">
         <v>89</v>
       </c>
@@ -11884,7 +11925,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="112" t="s">
         <v>89</v>
       </c>
@@ -11929,7 +11970,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="112" t="s">
         <v>87</v>
       </c>
@@ -11974,7 +12015,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="112" t="s">
         <v>97</v>
       </c>
@@ -12019,7 +12060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="112" t="s">
         <v>80</v>
       </c>
@@ -12066,7 +12107,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="112" t="s">
         <v>77</v>
       </c>
@@ -12111,7 +12152,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="112" t="s">
         <v>79</v>
       </c>
@@ -12156,7 +12197,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="112" t="s">
         <v>80</v>
       </c>
@@ -12201,7 +12242,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="112" t="s">
         <v>80</v>
       </c>
@@ -12246,7 +12287,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="112" t="s">
         <v>80</v>
       </c>
@@ -12293,7 +12334,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="112" t="s">
         <v>79</v>
       </c>
@@ -12338,7 +12379,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G48" s="115">
         <f>SUM(G2:G47)</f>
         <v>-82967225.110000014</v>
@@ -12349,8 +12390,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U1">
-    <sortState ref="A2:U49">
+  <autoFilter ref="A1:U1" xr:uid="{00000000-0009-0000-0000-000008000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U49">
       <sortCondition ref="P1"/>
     </sortState>
   </autoFilter>

</xml_diff>